<commit_message>
Starting formula runs and all PSC and all Proj for cust.
</commit_message>
<xml_diff>
--- a/Output/AcqTrends/Platform/Unlabeled/DoD_Unlabeled_Contracts.xlsx
+++ b/Output/AcqTrends/Platform/Unlabeled/DoD_Unlabeled_Contracts.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t xml:space="preserve">SimpleArea</t>
   </si>
@@ -214,19 +214,26 @@
   <si>
     <t xml:space="preserve">ProjectID</t>
   </si>
+  <si>
+    <t xml:space="preserve">Grand Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="7">
+  <numFmts count="8">
     <numFmt numFmtId="167" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="168" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="169" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="176" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="173" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="180" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="182" formatCode="0.00,,,&quot;B&quot;"/>
     <numFmt numFmtId="175" formatCode="0.00,,,&quot;B&quot;"/>
-    <numFmt numFmtId="177" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="181" formatCode="0.00,,,&quot;B&quot;"/>
+    <numFmt numFmtId="183" formatCode="0.00,,,&quot;B&quot;"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -262,15 +269,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="168" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="173" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="182" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
     <xf numFmtId="175" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="181" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="183" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4979,6 +4988,9 @@
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
+      <c r="A1" t="str">
+        <f>M1</f>
+      </c>
       <c r="M1" t="s">
         <v>58</v>
       </c>
@@ -5053,108 +5065,160 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="str">
+        <f>M2</f>
+      </c>
       <c r="M2"/>
-      <c r="N2" s="4" t="n">
+      <c r="N2" s="5" t="n">
         <v>29503352.0086</v>
       </c>
-      <c r="O2" s="4" t="n">
+      <c r="O2" s="5" t="n">
         <v>9825233.9429</v>
       </c>
-      <c r="P2" s="4" t="n">
+      <c r="P2" s="5" t="n">
         <v>84074351.1742</v>
       </c>
-      <c r="Q2" s="4" t="n">
+      <c r="Q2" s="5" t="n">
         <v>75741000.174</v>
       </c>
-      <c r="R2" s="4" t="n">
+      <c r="R2" s="5" t="n">
         <v>7078195.7826</v>
       </c>
-      <c r="S2" s="4" t="n">
+      <c r="S2" s="5" t="n">
         <v>3802636.1223</v>
       </c>
-      <c r="T2" s="4" t="n">
+      <c r="T2" s="5" t="n">
         <v>109748294.8077</v>
       </c>
-      <c r="U2" s="4" t="n">
+      <c r="U2" s="5" t="n">
         <v>18047585.0499</v>
       </c>
-      <c r="V2" s="4" t="n">
+      <c r="V2" s="5" t="n">
         <v>368043.2192</v>
       </c>
-      <c r="W2" s="4" t="n">
+      <c r="W2" s="5" t="n">
         <v>986168.1333</v>
       </c>
-      <c r="X2" s="4" t="n">
+      <c r="X2" s="5" t="n">
         <v>-253919.658</v>
       </c>
-      <c r="Y2" s="4" t="n">
+      <c r="Y2" s="5" t="n">
         <v>-140825.1013</v>
       </c>
-      <c r="Z2" s="4" t="n">
+      <c r="Z2" s="5" t="n">
         <v>-6477.8001</v>
       </c>
-      <c r="AA2" s="4" t="n">
+      <c r="AA2" s="5" t="n">
         <v>-99723.1206</v>
       </c>
-      <c r="AB2" s="4" t="n">
+      <c r="AB2" s="5" t="n">
         <v>30000</v>
       </c>
-      <c r="AC2" s="4" t="n">
+      <c r="AC2" s="5" t="n">
         <v>3581529.4308</v>
       </c>
-      <c r="AD2" s="4" t="n">
+      <c r="AD2" s="5" t="n">
         <v>1345607</v>
       </c>
-      <c r="AE2" s="4" t="n">
+      <c r="AE2" s="5" t="n">
         <v>-212795.3672</v>
       </c>
-      <c r="AF2" s="4" t="n">
+      <c r="AF2" s="5" t="n">
         <v>465885</v>
       </c>
-      <c r="AG2" s="4" t="n">
+      <c r="AG2" s="5" t="n">
         <v>314555.625</v>
       </c>
-      <c r="AH2" s="4" t="n">
+      <c r="AH2" s="5" t="n">
         <v>386316</v>
       </c>
-      <c r="AI2" s="4" t="n">
+      <c r="AI2" s="5" t="n">
         <v>980919.7685</v>
       </c>
-      <c r="AJ2" s="4" t="n">
+      <c r="AJ2" s="5" t="n">
         <v>335137.2418</v>
       </c>
-      <c r="AK2" s="4"/>
-      <c r="AL2" s="4"/>
+      <c r="AK2" s="5"/>
+      <c r="AL2" s="5"/>
     </row>
     <row r="3">
-      <c r="M3" t="str">
-        <f>Grand Total</f>
-      </c>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
-      <c r="Y3" s="4"/>
-      <c r="Z3" s="4"/>
-      <c r="AA3" s="4"/>
-      <c r="AB3" s="4"/>
-      <c r="AC3" s="4"/>
-      <c r="AD3" s="4"/>
-      <c r="AE3" s="4"/>
-      <c r="AF3" s="4"/>
-      <c r="AG3" s="4"/>
-      <c r="AH3" s="4"/>
-      <c r="AI3" s="4"/>
-      <c r="AJ3" s="4"/>
-      <c r="AK3" s="4"/>
-      <c r="AL3" s="4"/>
+      <c r="A3" t="str">
+        <f>M3</f>
+      </c>
+      <c r="M3" t="s">
+        <v>63</v>
+      </c>
+      <c r="N3" s="5" t="str">
+        <f>Sum(N2:N2)</f>
+      </c>
+      <c r="O3" s="5" t="str">
+        <f>Sum(O2:O2)</f>
+      </c>
+      <c r="P3" s="5" t="str">
+        <f>Sum(P2:P2)</f>
+      </c>
+      <c r="Q3" s="5" t="str">
+        <f>Sum(Q2:Q2)</f>
+      </c>
+      <c r="R3" s="5" t="str">
+        <f>Sum(R2:R2)</f>
+      </c>
+      <c r="S3" s="5" t="str">
+        <f>Sum(S2:S2)</f>
+      </c>
+      <c r="T3" s="5" t="str">
+        <f>Sum(T2:T2)</f>
+      </c>
+      <c r="U3" s="5" t="str">
+        <f>Sum(U2:U2)</f>
+      </c>
+      <c r="V3" s="5" t="str">
+        <f>Sum(V2:V2)</f>
+      </c>
+      <c r="W3" s="5" t="str">
+        <f>Sum(W2:W2)</f>
+      </c>
+      <c r="X3" s="5" t="str">
+        <f>Sum(X2:X2)</f>
+      </c>
+      <c r="Y3" s="5" t="str">
+        <f>Sum(Y2:Y2)</f>
+      </c>
+      <c r="Z3" s="5" t="str">
+        <f>Sum(Z2:Z2)</f>
+      </c>
+      <c r="AA3" s="5" t="str">
+        <f>Sum(AA2:AA2)</f>
+      </c>
+      <c r="AB3" s="5" t="str">
+        <f>Sum(AB2:AB2)</f>
+      </c>
+      <c r="AC3" s="5" t="str">
+        <f>Sum(AC2:AC2)</f>
+      </c>
+      <c r="AD3" s="5" t="str">
+        <f>Sum(AD2:AD2)</f>
+      </c>
+      <c r="AE3" s="5" t="str">
+        <f>Sum(AE2:AE2)</f>
+      </c>
+      <c r="AF3" s="5" t="str">
+        <f>Sum(AF2:AF2)</f>
+      </c>
+      <c r="AG3" s="5" t="str">
+        <f>Sum(AG2:AG2)</f>
+      </c>
+      <c r="AH3" s="5" t="str">
+        <f>Sum(AH2:AH2)</f>
+      </c>
+      <c r="AI3" s="5" t="str">
+        <f>Sum(AI2:AI2)</f>
+      </c>
+      <c r="AJ3" s="5" t="str">
+        <f>Sum(AJ2:AJ2)</f>
+      </c>
+      <c r="AK3" s="5"/>
+      <c r="AL3" s="5"/>
     </row>
     <row r="4">
       <c r="M4" t="str">
@@ -5167,6 +5231,36 @@
       </c>
     </row>
     <row r="6">
+      <c r="A6" t="str">
+        <f>M6</f>
+      </c>
+      <c r="B6" t="str">
+        <f>AB6</f>
+      </c>
+      <c r="C6" t="str">
+        <f>AH6</f>
+      </c>
+      <c r="D6" t="str">
+        <f>AI6</f>
+      </c>
+      <c r="E6" t="str">
+        <f>AJ6</f>
+      </c>
+      <c r="F6" t="str">
+        <f>AH6&amp;"-"&amp;AI6</f>
+      </c>
+      <c r="G6" t="str">
+        <f>AB6&amp;"-"&amp;AI6</f>
+      </c>
+      <c r="H6" t="str">
+        <f>AJ6&amp;"/"&amp;AI6</f>
+      </c>
+      <c r="I6" t="str">
+        <f>"Share "&amp;AI6</f>
+      </c>
+      <c r="J6" t="str">
+        <f>"Share "&amp;AJ6</f>
+      </c>
       <c r="M6" t="s">
         <v>58</v>
       </c>
@@ -5241,108 +5335,214 @@
       </c>
     </row>
     <row r="7">
+      <c r="A7" t="str">
+        <f>M7</f>
+      </c>
+      <c r="B7" s="5" t="str">
+        <f>AB7</f>
+      </c>
+      <c r="C7" s="5" t="str">
+        <f>AH7</f>
+      </c>
+      <c r="D7" s="5" t="str">
+        <f>AI7</f>
+      </c>
+      <c r="E7" s="5" t="str">
+        <f>AJ7</f>
+      </c>
+      <c r="F7" s="4" t="str">
+        <f>AI7/AH7-1</f>
+      </c>
+      <c r="G7" s="4" t="str">
+        <f>AI7/AB7-1</f>
+      </c>
+      <c r="H7" s="4" t="str">
+        <f>AJ7/AI7</f>
+      </c>
+      <c r="I7" s="4" t="str">
+        <f>AI7/Sum(AI$6:AI$7)</f>
+      </c>
+      <c r="J7" s="4" t="str">
+        <f>AJ7/Sum(AJ6:AJ$7)</f>
+      </c>
       <c r="M7"/>
-      <c r="N7" s="4" t="n">
+      <c r="N7" s="5" t="n">
         <v>47669452.4092127</v>
       </c>
-      <c r="O7" s="4" t="n">
+      <c r="O7" s="5" t="n">
         <v>15499081.938119</v>
       </c>
-      <c r="P7" s="4" t="n">
+      <c r="P7" s="5" t="n">
         <v>130564595.428863</v>
       </c>
-      <c r="Q7" s="4" t="n">
+      <c r="Q7" s="5" t="n">
         <v>115417039.647433</v>
       </c>
-      <c r="R7" s="4" t="n">
+      <c r="R7" s="5" t="n">
         <v>10528669.9110078</v>
       </c>
-      <c r="S7" s="4" t="n">
+      <c r="S7" s="5" t="n">
         <v>5489693.53365965</v>
       </c>
-      <c r="T7" s="4" t="n">
+      <c r="T7" s="5" t="n">
         <v>153442908.382779</v>
       </c>
-      <c r="U7" s="4" t="n">
+      <c r="U7" s="5" t="n">
         <v>24559459.5326898</v>
       </c>
-      <c r="V7" s="4" t="n">
+      <c r="V7" s="5" t="n">
         <v>490607.415843205</v>
       </c>
-      <c r="W7" s="4" t="n">
+      <c r="W7" s="5" t="n">
         <v>1301353.38051841</v>
       </c>
-      <c r="X7" s="4" t="n">
+      <c r="X7" s="5" t="n">
         <v>-332184.734254936</v>
       </c>
-      <c r="Y7" s="4" t="n">
+      <c r="Y7" s="5" t="n">
         <v>-180591.700596691</v>
       </c>
-      <c r="Z7" s="4" t="n">
+      <c r="Z7" s="5" t="n">
         <v>-8157.49366437355</v>
       </c>
-      <c r="AA7" s="4" t="n">
+      <c r="AA7" s="5" t="n">
         <v>-123324.487592803</v>
       </c>
-      <c r="AB7" s="4" t="n">
+      <c r="AB7" s="5" t="n">
         <v>35983.4270122674</v>
       </c>
-      <c r="AC7" s="4" t="n">
+      <c r="AC7" s="5" t="n">
         <v>4260551.68588794</v>
       </c>
-      <c r="AD7" s="4" t="n">
+      <c r="AD7" s="5" t="n">
         <v>1572643.0588818</v>
       </c>
-      <c r="AE7" s="4" t="n">
+      <c r="AE7" s="5" t="n">
         <v>-242993.47650284</v>
       </c>
-      <c r="AF7" s="4" t="n">
+      <c r="AF7" s="5" t="n">
         <v>521779.598543694</v>
       </c>
-      <c r="AG7" s="4" t="n">
+      <c r="AG7" s="5" t="n">
         <v>347656.572563343</v>
       </c>
-      <c r="AH7" s="4" t="n">
+      <c r="AH7" s="5" t="n">
         <v>413082.906520774</v>
       </c>
-      <c r="AI7" s="4" t="n">
+      <c r="AI7" s="5" t="n">
         <v>980919.7685</v>
       </c>
-      <c r="AJ7" s="4" t="n">
+      <c r="AJ7" s="5" t="n">
         <v>319653.358117263</v>
       </c>
-      <c r="AK7" s="4"/>
-      <c r="AL7" s="4"/>
+      <c r="AK7" s="5"/>
+      <c r="AL7" s="5"/>
     </row>
     <row r="8">
-      <c r="M8" t="str">
-        <f>Grand Total</f>
-      </c>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
-      <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
-      <c r="T8" s="4"/>
-      <c r="U8" s="4"/>
-      <c r="V8" s="4"/>
-      <c r="W8" s="4"/>
-      <c r="X8" s="4"/>
-      <c r="Y8" s="4"/>
-      <c r="Z8" s="4"/>
-      <c r="AA8" s="4"/>
-      <c r="AB8" s="4"/>
-      <c r="AC8" s="4"/>
-      <c r="AD8" s="4"/>
-      <c r="AE8" s="4"/>
-      <c r="AF8" s="4"/>
-      <c r="AG8" s="4"/>
-      <c r="AH8" s="4"/>
-      <c r="AI8" s="4"/>
-      <c r="AJ8" s="4"/>
-      <c r="AK8" s="4"/>
-      <c r="AL8" s="4"/>
+      <c r="A8" t="str">
+        <f>M8</f>
+      </c>
+      <c r="B8" s="5" t="str">
+        <f>AB8</f>
+      </c>
+      <c r="C8" s="5" t="str">
+        <f>AH8</f>
+      </c>
+      <c r="D8" s="5" t="str">
+        <f>AI8</f>
+      </c>
+      <c r="E8" s="5" t="str">
+        <f>AJ8</f>
+      </c>
+      <c r="F8" s="4" t="str">
+        <f>AI8/AH8-1</f>
+      </c>
+      <c r="G8" s="4" t="str">
+        <f>AI8/AB8-1</f>
+      </c>
+      <c r="H8" s="4" t="str">
+        <f>AJ8/AI8</f>
+      </c>
+      <c r="I8" s="4" t="str">
+        <f>Sum(I$6:I$7)</f>
+      </c>
+      <c r="J8" s="4" t="str">
+        <f>Sum(J$6:J$7)</f>
+      </c>
+      <c r="M8" t="s">
+        <v>63</v>
+      </c>
+      <c r="N8" s="5" t="str">
+        <f>Sum(N7:N7)</f>
+      </c>
+      <c r="O8" s="5" t="str">
+        <f>Sum(O7:O7)</f>
+      </c>
+      <c r="P8" s="5" t="str">
+        <f>Sum(P7:P7)</f>
+      </c>
+      <c r="Q8" s="5" t="str">
+        <f>Sum(Q7:Q7)</f>
+      </c>
+      <c r="R8" s="5" t="str">
+        <f>Sum(R7:R7)</f>
+      </c>
+      <c r="S8" s="5" t="str">
+        <f>Sum(S7:S7)</f>
+      </c>
+      <c r="T8" s="5" t="str">
+        <f>Sum(T7:T7)</f>
+      </c>
+      <c r="U8" s="5" t="str">
+        <f>Sum(U7:U7)</f>
+      </c>
+      <c r="V8" s="5" t="str">
+        <f>Sum(V7:V7)</f>
+      </c>
+      <c r="W8" s="5" t="str">
+        <f>Sum(W7:W7)</f>
+      </c>
+      <c r="X8" s="5" t="str">
+        <f>Sum(X7:X7)</f>
+      </c>
+      <c r="Y8" s="5" t="str">
+        <f>Sum(Y7:Y7)</f>
+      </c>
+      <c r="Z8" s="5" t="str">
+        <f>Sum(Z7:Z7)</f>
+      </c>
+      <c r="AA8" s="5" t="str">
+        <f>Sum(AA7:AA7)</f>
+      </c>
+      <c r="AB8" s="5" t="str">
+        <f>Sum(AB7:AB7)</f>
+      </c>
+      <c r="AC8" s="5" t="str">
+        <f>Sum(AC7:AC7)</f>
+      </c>
+      <c r="AD8" s="5" t="str">
+        <f>Sum(AD7:AD7)</f>
+      </c>
+      <c r="AE8" s="5" t="str">
+        <f>Sum(AE7:AE7)</f>
+      </c>
+      <c r="AF8" s="5" t="str">
+        <f>Sum(AF7:AF7)</f>
+      </c>
+      <c r="AG8" s="5" t="str">
+        <f>Sum(AG7:AG7)</f>
+      </c>
+      <c r="AH8" s="5" t="str">
+        <f>Sum(AH7:AH7)</f>
+      </c>
+      <c r="AI8" s="5" t="str">
+        <f>Sum(AI7:AI7)</f>
+      </c>
+      <c r="AJ8" s="5" t="str">
+        <f>Sum(AJ7:AJ7)</f>
+      </c>
+      <c r="AK8" s="5"/>
+      <c r="AL8" s="5"/>
     </row>
     <row r="9">
       <c r="M9" t="str">
@@ -5412,6 +5612,9 @@
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
+      <c r="A1" t="str">
+        <f>M1</f>
+      </c>
       <c r="M1" t="s">
         <v>59</v>
       </c>
@@ -5486,114 +5689,229 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="str">
+        <f>M2</f>
+      </c>
       <c r="M2" t="s">
         <v>60</v>
       </c>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="5"/>
-      <c r="AA2" s="5"/>
-      <c r="AB2" s="5"/>
-      <c r="AC2" s="5"/>
-      <c r="AD2" s="5"/>
-      <c r="AE2" s="5"/>
-      <c r="AF2" s="5"/>
-      <c r="AG2" s="5"/>
-      <c r="AH2" s="5"/>
-      <c r="AI2" s="5" t="n">
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+      <c r="AA2" s="6"/>
+      <c r="AB2" s="6"/>
+      <c r="AC2" s="6"/>
+      <c r="AD2" s="6"/>
+      <c r="AE2" s="6"/>
+      <c r="AF2" s="6"/>
+      <c r="AG2" s="6"/>
+      <c r="AH2" s="6"/>
+      <c r="AI2" s="6" t="n">
         <v>980919.7685</v>
       </c>
-      <c r="AJ2" s="5" t="n">
+      <c r="AJ2" s="6" t="n">
         <v>325137.2418</v>
       </c>
-      <c r="AK2" s="5"/>
-      <c r="AL2" s="5"/>
+      <c r="AK2" s="6"/>
+      <c r="AL2" s="6"/>
     </row>
     <row r="3">
+      <c r="A3" t="str">
+        <f>M3</f>
+      </c>
       <c r="M3"/>
-      <c r="N3" s="5" t="n">
+      <c r="N3" s="6" t="n">
         <v>29503352.0086</v>
       </c>
-      <c r="O3" s="5" t="n">
+      <c r="O3" s="6" t="n">
         <v>9825233.9429</v>
       </c>
-      <c r="P3" s="5" t="n">
+      <c r="P3" s="6" t="n">
         <v>84074351.1742</v>
       </c>
-      <c r="Q3" s="5" t="n">
+      <c r="Q3" s="6" t="n">
         <v>75741000.174</v>
       </c>
-      <c r="R3" s="5" t="n">
+      <c r="R3" s="6" t="n">
         <v>7078195.7826</v>
       </c>
-      <c r="S3" s="5" t="n">
+      <c r="S3" s="6" t="n">
         <v>3802636.1223</v>
       </c>
-      <c r="T3" s="5" t="n">
+      <c r="T3" s="6" t="n">
         <v>109748294.8077</v>
       </c>
-      <c r="U3" s="5" t="n">
+      <c r="U3" s="6" t="n">
         <v>18047585.0499</v>
       </c>
-      <c r="V3" s="5" t="n">
+      <c r="V3" s="6" t="n">
         <v>368043.2192</v>
       </c>
-      <c r="W3" s="5" t="n">
+      <c r="W3" s="6" t="n">
         <v>986168.1333</v>
       </c>
-      <c r="X3" s="5" t="n">
+      <c r="X3" s="6" t="n">
         <v>-253919.658</v>
       </c>
-      <c r="Y3" s="5" t="n">
+      <c r="Y3" s="6" t="n">
         <v>-140825.1013</v>
       </c>
-      <c r="Z3" s="5" t="n">
+      <c r="Z3" s="6" t="n">
         <v>-6477.8001</v>
       </c>
-      <c r="AA3" s="5" t="n">
+      <c r="AA3" s="6" t="n">
         <v>-99723.1206</v>
       </c>
-      <c r="AB3" s="5" t="n">
+      <c r="AB3" s="6" t="n">
         <v>30000</v>
       </c>
-      <c r="AC3" s="5" t="n">
+      <c r="AC3" s="6" t="n">
         <v>3581529.4308</v>
       </c>
-      <c r="AD3" s="5" t="n">
+      <c r="AD3" s="6" t="n">
         <v>1345607</v>
       </c>
-      <c r="AE3" s="5" t="n">
+      <c r="AE3" s="6" t="n">
         <v>-212795.3672</v>
       </c>
-      <c r="AF3" s="5" t="n">
+      <c r="AF3" s="6" t="n">
         <v>465885</v>
       </c>
-      <c r="AG3" s="5" t="n">
+      <c r="AG3" s="6" t="n">
         <v>314555.625</v>
       </c>
-      <c r="AH3" s="5" t="n">
+      <c r="AH3" s="6" t="n">
         <v>386316</v>
       </c>
-      <c r="AI3" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="5" t="n">
+      <c r="AI3" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="6" t="n">
         <v>10000</v>
       </c>
-      <c r="AK3" s="5"/>
-      <c r="AL3" s="5"/>
+      <c r="AK3" s="6"/>
+      <c r="AL3" s="6"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <f>M4</f>
+      </c>
+      <c r="M4" t="s">
+        <v>63</v>
+      </c>
+      <c r="N4" s="6" t="str">
+        <f>Sum(N2:N3)</f>
+      </c>
+      <c r="O4" s="6" t="str">
+        <f>Sum(O2:O3)</f>
+      </c>
+      <c r="P4" s="6" t="str">
+        <f>Sum(P2:P3)</f>
+      </c>
+      <c r="Q4" s="6" t="str">
+        <f>Sum(Q2:Q3)</f>
+      </c>
+      <c r="R4" s="6" t="str">
+        <f>Sum(R2:R3)</f>
+      </c>
+      <c r="S4" s="6" t="str">
+        <f>Sum(S2:S3)</f>
+      </c>
+      <c r="T4" s="6" t="str">
+        <f>Sum(T2:T3)</f>
+      </c>
+      <c r="U4" s="6" t="str">
+        <f>Sum(U2:U3)</f>
+      </c>
+      <c r="V4" s="6" t="str">
+        <f>Sum(V2:V3)</f>
+      </c>
+      <c r="W4" s="6" t="str">
+        <f>Sum(W2:W3)</f>
+      </c>
+      <c r="X4" s="6" t="str">
+        <f>Sum(X2:X3)</f>
+      </c>
+      <c r="Y4" s="6" t="str">
+        <f>Sum(Y2:Y3)</f>
+      </c>
+      <c r="Z4" s="6" t="str">
+        <f>Sum(Z2:Z3)</f>
+      </c>
+      <c r="AA4" s="6" t="str">
+        <f>Sum(AA2:AA3)</f>
+      </c>
+      <c r="AB4" s="6" t="str">
+        <f>Sum(AB2:AB3)</f>
+      </c>
+      <c r="AC4" s="6" t="str">
+        <f>Sum(AC2:AC3)</f>
+      </c>
+      <c r="AD4" s="6" t="str">
+        <f>Sum(AD2:AD3)</f>
+      </c>
+      <c r="AE4" s="6" t="str">
+        <f>Sum(AE2:AE3)</f>
+      </c>
+      <c r="AF4" s="6" t="str">
+        <f>Sum(AF2:AF3)</f>
+      </c>
+      <c r="AG4" s="6" t="str">
+        <f>Sum(AG2:AG3)</f>
+      </c>
+      <c r="AH4" s="6" t="str">
+        <f>Sum(AH2:AH3)</f>
+      </c>
+      <c r="AI4" s="6" t="str">
+        <f>Sum(AI2:AI3)</f>
+      </c>
+      <c r="AJ4" s="6" t="str">
+        <f>Sum(AJ2:AJ3)</f>
+      </c>
+      <c r="AK4" s="6"/>
+      <c r="AL4" s="6"/>
     </row>
     <row r="7">
+      <c r="A7" t="str">
+        <f>M7</f>
+      </c>
+      <c r="B7" t="str">
+        <f>AB7</f>
+      </c>
+      <c r="C7" t="str">
+        <f>AH7</f>
+      </c>
+      <c r="D7" t="str">
+        <f>AI7</f>
+      </c>
+      <c r="E7" t="str">
+        <f>AJ7</f>
+      </c>
+      <c r="F7" t="str">
+        <f>AH7&amp;"-"&amp;AI7</f>
+      </c>
+      <c r="G7" t="str">
+        <f>AB7&amp;"-"&amp;AI7</f>
+      </c>
+      <c r="H7" t="str">
+        <f>AJ7&amp;"/"&amp;AI7</f>
+      </c>
+      <c r="I7" t="str">
+        <f>"Share "&amp;AI7</f>
+      </c>
+      <c r="J7" t="str">
+        <f>"Share "&amp;AJ7</f>
+      </c>
       <c r="M7" t="s">
         <v>59</v>
       </c>
@@ -5668,112 +5986,278 @@
       </c>
     </row>
     <row r="8">
+      <c r="A8" t="str">
+        <f>M8</f>
+      </c>
+      <c r="B8" s="6" t="str">
+        <f>AB8</f>
+      </c>
+      <c r="C8" s="6" t="str">
+        <f>AH8</f>
+      </c>
+      <c r="D8" s="6" t="str">
+        <f>AI8</f>
+      </c>
+      <c r="E8" s="6" t="str">
+        <f>AJ8</f>
+      </c>
+      <c r="F8" s="4" t="str">
+        <f>AI8/AH8-1</f>
+      </c>
+      <c r="G8" s="4" t="str">
+        <f>AI8/AB8-1</f>
+      </c>
+      <c r="H8" s="4" t="str">
+        <f>AJ8/AI8</f>
+      </c>
+      <c r="I8" s="4" t="str">
+        <f>AI8/Sum(AI$7:AI$9)</f>
+      </c>
+      <c r="J8" s="4" t="str">
+        <f>AJ8/Sum(AJ7:AJ$9)</f>
+      </c>
       <c r="M8" t="s">
         <v>60</v>
       </c>
-      <c r="N8" s="5"/>
-      <c r="O8" s="5"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5"/>
-      <c r="U8" s="5"/>
-      <c r="V8" s="5"/>
-      <c r="W8" s="5"/>
-      <c r="X8" s="5"/>
-      <c r="Y8" s="5"/>
-      <c r="Z8" s="5"/>
-      <c r="AA8" s="5"/>
-      <c r="AB8" s="5"/>
-      <c r="AC8" s="5"/>
-      <c r="AD8" s="5"/>
-      <c r="AE8" s="5"/>
-      <c r="AF8" s="5"/>
-      <c r="AG8" s="5"/>
-      <c r="AH8" s="5"/>
-      <c r="AI8" s="5" t="n">
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="6"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6"/>
+      <c r="AE8" s="6"/>
+      <c r="AF8" s="6"/>
+      <c r="AG8" s="6"/>
+      <c r="AH8" s="6"/>
+      <c r="AI8" s="6" t="n">
         <v>980919.7685</v>
       </c>
-      <c r="AJ8" s="5" t="n">
+      <c r="AJ8" s="6" t="n">
         <v>310115.37432291</v>
       </c>
-      <c r="AK8" s="5"/>
-      <c r="AL8" s="5"/>
+      <c r="AK8" s="6"/>
+      <c r="AL8" s="6"/>
     </row>
     <row r="9">
+      <c r="A9" t="str">
+        <f>M9</f>
+      </c>
+      <c r="B9" s="6" t="str">
+        <f>AB9</f>
+      </c>
+      <c r="C9" s="6" t="str">
+        <f>AH9</f>
+      </c>
+      <c r="D9" s="6" t="str">
+        <f>AI9</f>
+      </c>
+      <c r="E9" s="6" t="str">
+        <f>AJ9</f>
+      </c>
+      <c r="F9" s="4" t="str">
+        <f>AI9/AH9-1</f>
+      </c>
+      <c r="G9" s="4" t="str">
+        <f>AI9/AB9-1</f>
+      </c>
+      <c r="H9" s="4" t="str">
+        <f>AJ9/AI9</f>
+      </c>
+      <c r="I9" s="4" t="str">
+        <f>AI9/Sum(AI$7:AI$9)</f>
+      </c>
+      <c r="J9" s="4" t="str">
+        <f>AJ9/Sum(AJ7:AJ$9)</f>
+      </c>
       <c r="M9"/>
-      <c r="N9" s="5" t="n">
+      <c r="N9" s="6" t="n">
         <v>47669452.4092127</v>
       </c>
-      <c r="O9" s="5" t="n">
+      <c r="O9" s="6" t="n">
         <v>15499081.938119</v>
       </c>
-      <c r="P9" s="5" t="n">
+      <c r="P9" s="6" t="n">
         <v>130564595.428863</v>
       </c>
-      <c r="Q9" s="5" t="n">
+      <c r="Q9" s="6" t="n">
         <v>115417039.647433</v>
       </c>
-      <c r="R9" s="5" t="n">
+      <c r="R9" s="6" t="n">
         <v>10528669.9110078</v>
       </c>
-      <c r="S9" s="5" t="n">
+      <c r="S9" s="6" t="n">
         <v>5489693.53365965</v>
       </c>
-      <c r="T9" s="5" t="n">
+      <c r="T9" s="6" t="n">
         <v>153442908.382779</v>
       </c>
-      <c r="U9" s="5" t="n">
+      <c r="U9" s="6" t="n">
         <v>24559459.5326898</v>
       </c>
-      <c r="V9" s="5" t="n">
+      <c r="V9" s="6" t="n">
         <v>490607.415843205</v>
       </c>
-      <c r="W9" s="5" t="n">
+      <c r="W9" s="6" t="n">
         <v>1301353.38051841</v>
       </c>
-      <c r="X9" s="5" t="n">
+      <c r="X9" s="6" t="n">
         <v>-332184.734254936</v>
       </c>
-      <c r="Y9" s="5" t="n">
+      <c r="Y9" s="6" t="n">
         <v>-180591.700596691</v>
       </c>
-      <c r="Z9" s="5" t="n">
+      <c r="Z9" s="6" t="n">
         <v>-8157.49366437355</v>
       </c>
-      <c r="AA9" s="5" t="n">
+      <c r="AA9" s="6" t="n">
         <v>-123324.487592803</v>
       </c>
-      <c r="AB9" s="5" t="n">
+      <c r="AB9" s="6" t="n">
         <v>35983.4270122674</v>
       </c>
-      <c r="AC9" s="5" t="n">
+      <c r="AC9" s="6" t="n">
         <v>4260551.68588794</v>
       </c>
-      <c r="AD9" s="5" t="n">
+      <c r="AD9" s="6" t="n">
         <v>1572643.0588818</v>
       </c>
-      <c r="AE9" s="5" t="n">
+      <c r="AE9" s="6" t="n">
         <v>-242993.47650284</v>
       </c>
-      <c r="AF9" s="5" t="n">
+      <c r="AF9" s="6" t="n">
         <v>521779.598543694</v>
       </c>
-      <c r="AG9" s="5" t="n">
+      <c r="AG9" s="6" t="n">
         <v>347656.572563343</v>
       </c>
-      <c r="AH9" s="5" t="n">
+      <c r="AH9" s="6" t="n">
         <v>413082.906520774</v>
       </c>
-      <c r="AI9" s="5" t="n">
-        <v>0</v>
-      </c>
-      <c r="AJ9" s="5" t="n">
+      <c r="AI9" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="6" t="n">
         <v>9537.98379435319</v>
       </c>
-      <c r="AK9" s="5"/>
-      <c r="AL9" s="5"/>
+      <c r="AK9" s="6"/>
+      <c r="AL9" s="6"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <f>M10</f>
+      </c>
+      <c r="B10" s="6" t="str">
+        <f>AB10</f>
+      </c>
+      <c r="C10" s="6" t="str">
+        <f>AH10</f>
+      </c>
+      <c r="D10" s="6" t="str">
+        <f>AI10</f>
+      </c>
+      <c r="E10" s="6" t="str">
+        <f>AJ10</f>
+      </c>
+      <c r="F10" s="4" t="str">
+        <f>AI10/AH10-1</f>
+      </c>
+      <c r="G10" s="4" t="str">
+        <f>AI10/AB10-1</f>
+      </c>
+      <c r="H10" s="4" t="str">
+        <f>AJ10/AI10</f>
+      </c>
+      <c r="I10" s="4" t="str">
+        <f>Sum(I$7:I$9)</f>
+      </c>
+      <c r="J10" s="4" t="str">
+        <f>Sum(J$7:J$9)</f>
+      </c>
+      <c r="M10" t="s">
+        <v>63</v>
+      </c>
+      <c r="N10" s="6" t="str">
+        <f>Sum(N8:N9)</f>
+      </c>
+      <c r="O10" s="6" t="str">
+        <f>Sum(O8:O9)</f>
+      </c>
+      <c r="P10" s="6" t="str">
+        <f>Sum(P8:P9)</f>
+      </c>
+      <c r="Q10" s="6" t="str">
+        <f>Sum(Q8:Q9)</f>
+      </c>
+      <c r="R10" s="6" t="str">
+        <f>Sum(R8:R9)</f>
+      </c>
+      <c r="S10" s="6" t="str">
+        <f>Sum(S8:S9)</f>
+      </c>
+      <c r="T10" s="6" t="str">
+        <f>Sum(T8:T9)</f>
+      </c>
+      <c r="U10" s="6" t="str">
+        <f>Sum(U8:U9)</f>
+      </c>
+      <c r="V10" s="6" t="str">
+        <f>Sum(V8:V9)</f>
+      </c>
+      <c r="W10" s="6" t="str">
+        <f>Sum(W8:W9)</f>
+      </c>
+      <c r="X10" s="6" t="str">
+        <f>Sum(X8:X9)</f>
+      </c>
+      <c r="Y10" s="6" t="str">
+        <f>Sum(Y8:Y9)</f>
+      </c>
+      <c r="Z10" s="6" t="str">
+        <f>Sum(Z8:Z9)</f>
+      </c>
+      <c r="AA10" s="6" t="str">
+        <f>Sum(AA8:AA9)</f>
+      </c>
+      <c r="AB10" s="6" t="str">
+        <f>Sum(AB8:AB9)</f>
+      </c>
+      <c r="AC10" s="6" t="str">
+        <f>Sum(AC8:AC9)</f>
+      </c>
+      <c r="AD10" s="6" t="str">
+        <f>Sum(AD8:AD9)</f>
+      </c>
+      <c r="AE10" s="6" t="str">
+        <f>Sum(AE8:AE9)</f>
+      </c>
+      <c r="AF10" s="6" t="str">
+        <f>Sum(AF8:AF9)</f>
+      </c>
+      <c r="AG10" s="6" t="str">
+        <f>Sum(AG8:AG9)</f>
+      </c>
+      <c r="AH10" s="6" t="str">
+        <f>Sum(AH8:AH9)</f>
+      </c>
+      <c r="AI10" s="6" t="str">
+        <f>Sum(AI8:AI9)</f>
+      </c>
+      <c r="AJ10" s="6" t="str">
+        <f>Sum(AJ8:AJ9)</f>
+      </c>
+      <c r="AK10" s="6"/>
+      <c r="AL10" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5872,76 +6356,76 @@
     <row r="2">
       <c r="M2"/>
       <c r="N2"/>
-      <c r="O2" s="6" t="n">
+      <c r="O2" s="7" t="n">
         <v>47669452.4092127</v>
       </c>
-      <c r="P2" s="6" t="n">
+      <c r="P2" s="7" t="n">
         <v>15499081.938119</v>
       </c>
-      <c r="Q2" s="6" t="n">
+      <c r="Q2" s="7" t="n">
         <v>130564595.428863</v>
       </c>
-      <c r="R2" s="6" t="n">
+      <c r="R2" s="7" t="n">
         <v>115417039.647433</v>
       </c>
-      <c r="S2" s="6" t="n">
+      <c r="S2" s="7" t="n">
         <v>10528669.9110078</v>
       </c>
-      <c r="T2" s="6" t="n">
+      <c r="T2" s="7" t="n">
         <v>5489693.53365965</v>
       </c>
-      <c r="U2" s="6" t="n">
+      <c r="U2" s="7" t="n">
         <v>153442908.382779</v>
       </c>
-      <c r="V2" s="6" t="n">
+      <c r="V2" s="7" t="n">
         <v>24559459.5326898</v>
       </c>
-      <c r="W2" s="6" t="n">
+      <c r="W2" s="7" t="n">
         <v>490607.415843205</v>
       </c>
-      <c r="X2" s="6" t="n">
+      <c r="X2" s="7" t="n">
         <v>1301353.38051841</v>
       </c>
-      <c r="Y2" s="6" t="n">
+      <c r="Y2" s="7" t="n">
         <v>-332184.734254936</v>
       </c>
-      <c r="Z2" s="6" t="n">
+      <c r="Z2" s="7" t="n">
         <v>-180591.700596691</v>
       </c>
-      <c r="AA2" s="6" t="n">
+      <c r="AA2" s="7" t="n">
         <v>-8157.49366437355</v>
       </c>
-      <c r="AB2" s="6" t="n">
+      <c r="AB2" s="7" t="n">
         <v>-123324.487592803</v>
       </c>
-      <c r="AC2" s="6" t="n">
+      <c r="AC2" s="7" t="n">
         <v>35983.4270122674</v>
       </c>
-      <c r="AD2" s="6" t="n">
+      <c r="AD2" s="7" t="n">
         <v>4260551.68588794</v>
       </c>
-      <c r="AE2" s="6" t="n">
+      <c r="AE2" s="7" t="n">
         <v>1572643.0588818</v>
       </c>
-      <c r="AF2" s="6" t="n">
+      <c r="AF2" s="7" t="n">
         <v>-242993.47650284</v>
       </c>
-      <c r="AG2" s="6" t="n">
+      <c r="AG2" s="7" t="n">
         <v>521779.598543694</v>
       </c>
-      <c r="AH2" s="6" t="n">
+      <c r="AH2" s="7" t="n">
         <v>347656.572563343</v>
       </c>
-      <c r="AI2" s="6" t="n">
+      <c r="AI2" s="7" t="n">
         <v>413082.906520774</v>
       </c>
-      <c r="AJ2" s="6" t="n">
+      <c r="AJ2" s="7" t="n">
         <v>980919.7685</v>
       </c>
-      <c r="AK2" s="6" t="n">
+      <c r="AK2" s="7" t="n">
         <v>319653.358117263</v>
       </c>
-      <c r="AL2" s="6"/>
+      <c r="AL2" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5961,6 +6445,39 @@
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
+      <c r="A1" t="str">
+        <f>O1</f>
+      </c>
+      <c r="B1" t="str">
+        <f>P1</f>
+      </c>
+      <c r="C1" t="str">
+        <f>AE1</f>
+      </c>
+      <c r="D1" t="str">
+        <f>AK1</f>
+      </c>
+      <c r="E1" t="str">
+        <f>AL1</f>
+      </c>
+      <c r="F1" t="str">
+        <f>AM1</f>
+      </c>
+      <c r="G1" t="str">
+        <f>AK1&amp;"-"&amp;AL1</f>
+      </c>
+      <c r="H1" t="str">
+        <f>AE1&amp;"-"&amp;AL1</f>
+      </c>
+      <c r="I1" t="str">
+        <f>AM1&amp;"/"&amp;AL1</f>
+      </c>
+      <c r="J1" t="str">
+        <f>"Share "&amp;AL1</f>
+      </c>
+      <c r="K1" t="str">
+        <f>"Share "&amp;AM1</f>
+      </c>
       <c r="O1" t="s">
         <v>61</v>
       </c>
@@ -6038,107 +6555,220 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="str">
+        <f>O2</f>
+      </c>
+      <c r="B2" t="str">
+        <f>P2</f>
+      </c>
+      <c r="C2" s="9" t="str">
+        <f>AE2</f>
+      </c>
+      <c r="D2" s="9" t="str">
+        <f>AK2</f>
+      </c>
+      <c r="E2" s="9" t="str">
+        <f>AL2</f>
+      </c>
+      <c r="F2" s="9" t="str">
+        <f>AM2</f>
+      </c>
+      <c r="G2" s="4" t="str">
+        <f>AL2/AK2-1</f>
+      </c>
+      <c r="H2" s="4" t="str">
+        <f>AL2/AE2-1</f>
+      </c>
+      <c r="I2" s="4" t="str">
+        <f>AM2/AL2</f>
+      </c>
+      <c r="J2" s="4" t="str">
+        <f>AL2/Sum(AL$1:AL$2)</f>
+      </c>
+      <c r="K2" s="4" t="str">
+        <f>AM2/Sum(AM1:AM$2)</f>
+      </c>
       <c r="O2"/>
       <c r="P2"/>
-      <c r="Q2" s="7" t="n">
+      <c r="Q2" s="9" t="n">
         <v>47669452.4092127</v>
       </c>
-      <c r="R2" s="7" t="n">
+      <c r="R2" s="9" t="n">
         <v>15499081.938119</v>
       </c>
-      <c r="S2" s="7" t="n">
+      <c r="S2" s="9" t="n">
         <v>130564595.428863</v>
       </c>
-      <c r="T2" s="7" t="n">
+      <c r="T2" s="9" t="n">
         <v>115417039.647433</v>
       </c>
-      <c r="U2" s="7" t="n">
+      <c r="U2" s="9" t="n">
         <v>10528669.9110078</v>
       </c>
-      <c r="V2" s="7" t="n">
+      <c r="V2" s="9" t="n">
         <v>5489693.53365965</v>
       </c>
-      <c r="W2" s="7" t="n">
+      <c r="W2" s="9" t="n">
         <v>153442908.382779</v>
       </c>
-      <c r="X2" s="7" t="n">
+      <c r="X2" s="9" t="n">
         <v>24559459.5326898</v>
       </c>
-      <c r="Y2" s="7" t="n">
+      <c r="Y2" s="9" t="n">
         <v>490607.415843205</v>
       </c>
-      <c r="Z2" s="7" t="n">
+      <c r="Z2" s="9" t="n">
         <v>1301353.38051841</v>
       </c>
-      <c r="AA2" s="7" t="n">
+      <c r="AA2" s="9" t="n">
         <v>-332184.734254936</v>
       </c>
-      <c r="AB2" s="7" t="n">
+      <c r="AB2" s="9" t="n">
         <v>-180591.700596691</v>
       </c>
-      <c r="AC2" s="7" t="n">
+      <c r="AC2" s="9" t="n">
         <v>-8157.49366437355</v>
       </c>
-      <c r="AD2" s="7" t="n">
+      <c r="AD2" s="9" t="n">
         <v>-123324.487592803</v>
       </c>
-      <c r="AE2" s="7" t="n">
+      <c r="AE2" s="9" t="n">
         <v>35983.4270122674</v>
       </c>
-      <c r="AF2" s="7" t="n">
+      <c r="AF2" s="9" t="n">
         <v>4260551.68588794</v>
       </c>
-      <c r="AG2" s="7" t="n">
+      <c r="AG2" s="9" t="n">
         <v>1572643.0588818</v>
       </c>
-      <c r="AH2" s="7" t="n">
+      <c r="AH2" s="9" t="n">
         <v>-242993.47650284</v>
       </c>
-      <c r="AI2" s="7" t="n">
+      <c r="AI2" s="9" t="n">
         <v>521779.598543694</v>
       </c>
-      <c r="AJ2" s="7" t="n">
+      <c r="AJ2" s="9" t="n">
         <v>347656.572563343</v>
       </c>
-      <c r="AK2" s="7" t="n">
+      <c r="AK2" s="9" t="n">
         <v>413082.906520774</v>
       </c>
-      <c r="AL2" s="7" t="n">
+      <c r="AL2" s="9" t="n">
         <v>980919.7685</v>
       </c>
-      <c r="AM2" s="7" t="n">
+      <c r="AM2" s="9" t="n">
         <v>319653.358117263</v>
       </c>
-      <c r="AN2" s="7"/>
+      <c r="AN2" s="9"/>
     </row>
     <row r="3">
-      <c r="P3" t="str">
-        <f>Grand Total</f>
-      </c>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
-      <c r="AA3" s="7"/>
-      <c r="AB3" s="7"/>
-      <c r="AC3" s="7"/>
-      <c r="AD3" s="7"/>
-      <c r="AE3" s="7"/>
-      <c r="AF3" s="7"/>
-      <c r="AG3" s="7"/>
-      <c r="AH3" s="7"/>
-      <c r="AI3" s="7"/>
-      <c r="AJ3" s="7"/>
-      <c r="AK3" s="7"/>
-      <c r="AL3" s="7"/>
-      <c r="AM3" s="7"/>
-      <c r="AN3" s="7"/>
+      <c r="A3" t="str">
+        <f>O3</f>
+      </c>
+      <c r="B3" t="str">
+        <f>P3</f>
+      </c>
+      <c r="C3" s="9" t="str">
+        <f>AE3</f>
+      </c>
+      <c r="D3" s="9" t="str">
+        <f>AK3</f>
+      </c>
+      <c r="E3" s="9" t="str">
+        <f>AL3</f>
+      </c>
+      <c r="F3" s="9" t="str">
+        <f>AM3</f>
+      </c>
+      <c r="G3" s="4" t="str">
+        <f>AL3/AK3-1</f>
+      </c>
+      <c r="H3" s="4" t="str">
+        <f>AL3/AE3-1</f>
+      </c>
+      <c r="I3" s="4" t="str">
+        <f>AM3/AL3</f>
+      </c>
+      <c r="J3" s="4" t="str">
+        <f>Sum(J$1:J$2)</f>
+      </c>
+      <c r="K3" s="4" t="str">
+        <f>Sum(K$1:K$2)</f>
+      </c>
+      <c r="O3" t="s">
+        <v>63</v>
+      </c>
+      <c r="P3" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q3" s="9" t="str">
+        <f>Sum(Q2:Q2)</f>
+      </c>
+      <c r="R3" s="9" t="str">
+        <f>Sum(R2:R2)</f>
+      </c>
+      <c r="S3" s="9" t="str">
+        <f>Sum(S2:S2)</f>
+      </c>
+      <c r="T3" s="9" t="str">
+        <f>Sum(T2:T2)</f>
+      </c>
+      <c r="U3" s="9" t="str">
+        <f>Sum(U2:U2)</f>
+      </c>
+      <c r="V3" s="9" t="str">
+        <f>Sum(V2:V2)</f>
+      </c>
+      <c r="W3" s="9" t="str">
+        <f>Sum(W2:W2)</f>
+      </c>
+      <c r="X3" s="9" t="str">
+        <f>Sum(X2:X2)</f>
+      </c>
+      <c r="Y3" s="9" t="str">
+        <f>Sum(Y2:Y2)</f>
+      </c>
+      <c r="Z3" s="9" t="str">
+        <f>Sum(Z2:Z2)</f>
+      </c>
+      <c r="AA3" s="9" t="str">
+        <f>Sum(AA2:AA2)</f>
+      </c>
+      <c r="AB3" s="9" t="str">
+        <f>Sum(AB2:AB2)</f>
+      </c>
+      <c r="AC3" s="9" t="str">
+        <f>Sum(AC2:AC2)</f>
+      </c>
+      <c r="AD3" s="9" t="str">
+        <f>Sum(AD2:AD2)</f>
+      </c>
+      <c r="AE3" s="9" t="str">
+        <f>Sum(AE2:AE2)</f>
+      </c>
+      <c r="AF3" s="9" t="str">
+        <f>Sum(AF2:AF2)</f>
+      </c>
+      <c r="AG3" s="9" t="str">
+        <f>Sum(AG2:AG2)</f>
+      </c>
+      <c r="AH3" s="9" t="str">
+        <f>Sum(AH2:AH2)</f>
+      </c>
+      <c r="AI3" s="9" t="str">
+        <f>Sum(AI2:AI2)</f>
+      </c>
+      <c r="AJ3" s="9" t="str">
+        <f>Sum(AJ2:AJ2)</f>
+      </c>
+      <c r="AK3" s="9" t="str">
+        <f>Sum(AK2:AK2)</f>
+      </c>
+      <c r="AL3" s="9" t="str">
+        <f>Sum(AL2:AL2)</f>
+      </c>
+      <c r="AM3" s="9"/>
+      <c r="AN3" s="9"/>
     </row>
     <row r="4">
       <c r="P4" t="str">

</xml_diff>